<commit_message>
Tentative es calc for Acarturk et al.
</commit_message>
<xml_diff>
--- a/ES calc/Descriptive coding scheme for group-based interventions (data) MHV.xlsx
+++ b/ES calc/Descriptive coding scheme for group-based interventions (data) MHV.xlsx
@@ -919,8 +919,8 @@
   <dimension ref="A1:BF20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB7" sqref="AB7"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,7 +2928,7 @@
         <v>2013</v>
       </c>
       <c r="C12" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D12" s="4">
         <v>73559907</v>
@@ -3104,7 +3104,7 @@
         <v>2021</v>
       </c>
       <c r="C13" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="4">
         <v>73494601</v>
@@ -3280,7 +3280,7 @@
         <v>2021</v>
       </c>
       <c r="C14" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D14" s="4">
         <v>73494601</v>
@@ -3456,7 +3456,7 @@
         <v>2013</v>
       </c>
       <c r="C15" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D15" s="4">
         <v>73559907</v>
@@ -3632,7 +3632,7 @@
         <v>2021</v>
       </c>
       <c r="C16" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" s="4">
         <v>73494601</v>
@@ -3808,7 +3808,7 @@
         <v>2013</v>
       </c>
       <c r="C17" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" s="4">
         <v>73559907</v>
@@ -3984,7 +3984,7 @@
         <v>2013</v>
       </c>
       <c r="C18" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" s="4">
         <v>73559907</v>
@@ -4160,7 +4160,7 @@
         <v>2013</v>
       </c>
       <c r="C19" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="4">
         <v>73559907</v>
@@ -4336,7 +4336,7 @@
         <v>2013</v>
       </c>
       <c r="C20" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D20" s="4">
         <v>73559907</v>

</xml_diff>